<commit_message>
Commit2:Change in Input excel file
</commit_message>
<xml_diff>
--- a/GK_RF_Frame1/Input_Data/Inputs.xlsx
+++ b/GK_RF_Frame1/Input_Data/Inputs.xlsx
@@ -109,10 +109,10 @@
     <t>Member76</t>
   </si>
   <si>
-    <t>Mem81</t>
-  </si>
-  <si>
-    <t>Member81</t>
+    <t>Mem82</t>
+  </si>
+  <si>
+    <t>Member82</t>
   </si>
 </sst>
 </file>
@@ -517,7 +517,7 @@
   <dimension ref="A1:B3"/>
   <sheetViews>
     <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="80" zoomScaleNormal="80" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B15" activeCellId="0" sqref="B15"/>
+      <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>

</xml_diff>